<commit_message>
Add regslv rtl testbench for smoke verification
</commit_message>
<xml_diff>
--- a/parsers/excel/templates/template_cn.xlsx
+++ b/parsers/excel/templates/template_cn.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hj-micro\regslv\parser\excel\templates\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\hj-micro\Register Automation\regslv\parsers\excel\templates\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3FA6761-D5B3-416C-A667-091EACF7D528}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9FBD4406-2C8A-4EBD-8631-C0C6B2DF2E3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4212" yWindow="1908" windowWidth="22776" windowHeight="14652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4296" yWindow="900" windowWidth="22776" windowHeight="14652" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="TEM" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="39">
   <si>
     <t>名称</t>
   </si>
@@ -49,9 +49,6 @@
     <t>复位值</t>
   </si>
   <si>
-    <t>复位信号</t>
-  </si>
-  <si>
     <t>31:18</t>
   </si>
   <si>
@@ -62,9 +59,6 @@
   </si>
   <si>
     <t>0x0</t>
-  </si>
-  <si>
-    <t>Global Reset</t>
   </si>
   <si>
     <t>17:17</t>
@@ -131,10 +125,6 @@
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
   <si>
-    <t>RUSER</t>
-    <phoneticPr fontId="2" type="noConversion"/>
-  </si>
-  <si>
     <t>WOSET</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
@@ -152,6 +142,22 @@
   </si>
   <si>
     <t>TEM</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>同步复位信号</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>None</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>srst_10, srst_11</t>
+    <phoneticPr fontId="2" type="noConversion"/>
+  </si>
+  <si>
+    <t>srst_20</t>
     <phoneticPr fontId="2" type="noConversion"/>
   </si>
 </sst>
@@ -583,7 +589,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="9" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
@@ -596,7 +602,7 @@
         <v>1</v>
       </c>
       <c r="B2" s="9" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C2" s="10"/>
       <c r="D2" s="10"/>
@@ -606,7 +612,7 @@
     </row>
     <row r="3" spans="1:7" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A3" s="8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B3" s="11">
         <v>32</v>
@@ -654,131 +660,131 @@
         <v>4</v>
       </c>
       <c r="D8" s="6" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="E8" s="6" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F8" s="7" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="7" t="s">
-        <v>9</v>
+      <c r="G8" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B9" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="C9" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="D9" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E9" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E9" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="G9" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B10" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="3" t="s">
-        <v>17</v>
-      </c>
       <c r="D10" s="2" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="F10" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G10" s="2" t="s">
-        <v>14</v>
+        <v>37</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A11" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B11" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>20</v>
-      </c>
       <c r="D11" s="2" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="F11" s="2" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>14</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="100.05" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A12" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="F12" s="2" t="s">
         <v>21</v>
       </c>
-      <c r="B12" s="2" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="F12" s="2" t="s">
-        <v>23</v>
-      </c>
       <c r="G12" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A13" s="2" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B13" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C13" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="D13" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F13" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="F13" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="G13" s="2" t="s">
-        <v>14</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>